<commit_message>
Procx fim + corresp init
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/9.PROCX/2.PROCX_duplo_triplo.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/9.PROCX/2.PROCX_duplo_triplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\9.PROCX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B7B8A9-2E9A-4251-9B56-F832A897B91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75998B9-E8AB-44DA-85D6-4834E83FEBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12264" yWindow="120" windowWidth="10800" windowHeight="12792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D405"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>